<commit_message>
datos actuales 2 ts
</commit_message>
<xml_diff>
--- a/info/data2.xlsx
+++ b/info/data2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\ITESO\Traiding\Lab_4_Proyecto\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8525C127-8458-4990-A865-2A1EB6417E4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8C5832-7BF2-4E22-8238-3A9C04B9D524}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="1500" windowWidth="16560" windowHeight="9420" activeTab="1" xr2:uid="{EED82211-3F45-4361-BAEE-0972454E4BF2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{EED82211-3F45-4361-BAEE-0972454E4BF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -34,483 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="191">
   <si>
-    <t>04/17/2020 (Mar)</t>
-  </si>
-  <si>
-    <t>03/18/2020 (Feb)</t>
-  </si>
-  <si>
-    <t>02/21/2020 (Jan)</t>
-  </si>
-  <si>
-    <t>01/17/2020 (Dec)</t>
-  </si>
-  <si>
-    <t>12/18/2019 (Nov)</t>
-  </si>
-  <si>
-    <t>11/15/2019 (Oct)</t>
-  </si>
-  <si>
-    <t>10/16/2019 (Sep)</t>
-  </si>
-  <si>
-    <t>09/18/2019 (Aug)</t>
-  </si>
-  <si>
-    <t>08/19/2019 (Jul)</t>
-  </si>
-  <si>
-    <t>07/17/2019 (Jun)</t>
-  </si>
-  <si>
-    <t>06/18/2019 (May)</t>
-  </si>
-  <si>
-    <t>05/17/2019 (Apr)</t>
-  </si>
-  <si>
-    <t>04/17/2019 (Mar)</t>
-  </si>
-  <si>
-    <t>03/15/2019 (Feb)</t>
-  </si>
-  <si>
-    <t>02/22/2019 (Jan)</t>
-  </si>
-  <si>
-    <t>01/17/2019 (Dec)</t>
-  </si>
-  <si>
-    <t>12/17/2018 (Nov)</t>
-  </si>
-  <si>
-    <t>11/16/2018 (Oct)</t>
-  </si>
-  <si>
-    <t>10/17/2018 (Sep)</t>
-  </si>
-  <si>
-    <t>09/17/2018 (Aug)</t>
-  </si>
-  <si>
-    <t>08/17/2018 (Jul)</t>
-  </si>
-  <si>
-    <t>07/18/2018 (Jun)</t>
-  </si>
-  <si>
-    <t>06/15/2018 (May)</t>
-  </si>
-  <si>
-    <t>05/16/2018 (Apr)</t>
-  </si>
-  <si>
-    <t>04/18/2018 (Mar)</t>
-  </si>
-  <si>
-    <t>03/16/2018 (Feb)</t>
-  </si>
-  <si>
-    <t>02/23/2018 (Jan)</t>
-  </si>
-  <si>
-    <t>01/17/2018 (Dec)</t>
-  </si>
-  <si>
-    <t>12/18/2017 (Nov)</t>
-  </si>
-  <si>
-    <t>11/16/2017 (Oct)</t>
-  </si>
-  <si>
-    <t>10/17/2017 (Sep)</t>
-  </si>
-  <si>
-    <t>09/18/2017 (Aug)</t>
-  </si>
-  <si>
-    <t>08/17/2017 (Jul)</t>
-  </si>
-  <si>
-    <t>07/17/2017 (Jun)</t>
-  </si>
-  <si>
-    <t>06/16/2017 (May)</t>
-  </si>
-  <si>
-    <t>05/17/2017 (Apr)</t>
-  </si>
-  <si>
-    <t>04/19/2017 (Mar)</t>
-  </si>
-  <si>
-    <t>03/16/2017 (Feb)</t>
-  </si>
-  <si>
-    <t>02/22/2017 (Jan)</t>
-  </si>
-  <si>
-    <t>01/18/2017 (Dec)</t>
-  </si>
-  <si>
-    <t>12/16/2016 (Nov)</t>
-  </si>
-  <si>
-    <t>11/17/2016 (Oct)</t>
-  </si>
-  <si>
-    <t>10/17/2016 (Sep)</t>
-  </si>
-  <si>
-    <t>09/15/2016 (Aug)</t>
-  </si>
-  <si>
-    <t>08/18/2016 (Jul)</t>
-  </si>
-  <si>
-    <t>07/15/2016 (Jun)</t>
-  </si>
-  <si>
-    <t>06/16/2016 (May)</t>
-  </si>
-  <si>
-    <t>05/18/2016 (Apr)</t>
-  </si>
-  <si>
-    <t>04/14/2016 (Mar)</t>
-  </si>
-  <si>
-    <t>03/17/2016 (Feb)</t>
-  </si>
-  <si>
-    <t>02/25/2016 (Jan)</t>
-  </si>
-  <si>
-    <t>01/19/2016 (Dec)</t>
-  </si>
-  <si>
-    <t>12/16/2015 (Nov)</t>
-  </si>
-  <si>
-    <t>11/16/2015 (Oct)</t>
-  </si>
-  <si>
-    <t>10/16/2015 (Sep)</t>
-  </si>
-  <si>
-    <t>09/16/2015 (Aug)</t>
-  </si>
-  <si>
-    <t>08/14/2015 (Jul)</t>
-  </si>
-  <si>
-    <t>07/16/2015 (Jun)</t>
-  </si>
-  <si>
-    <t>06/17/2015 (May)</t>
-  </si>
-  <si>
-    <t>05/19/2015 (Apr)</t>
-  </si>
-  <si>
-    <t>04/17/2015 (Mar)</t>
-  </si>
-  <si>
-    <t>03/17/2015 (Feb)</t>
-  </si>
-  <si>
-    <t>02/24/2015 (Jan)</t>
-  </si>
-  <si>
-    <t>01/16/2015 (Dec)</t>
-  </si>
-  <si>
-    <t>12/17/2014 (Nov)</t>
-  </si>
-  <si>
-    <t>11/14/2014 (Oct)</t>
-  </si>
-  <si>
-    <t>10/16/2014 (Sep)</t>
-  </si>
-  <si>
-    <t>09/17/2014 (Aug)</t>
-  </si>
-  <si>
-    <t>08/14/2014 (Jul)</t>
-  </si>
-  <si>
-    <t>07/17/2014 (Jun)</t>
-  </si>
-  <si>
-    <t>06/16/2014 (May)</t>
-  </si>
-  <si>
-    <t>05/15/2014 (Apr)</t>
-  </si>
-  <si>
-    <t>04/16/2014 (Mar)</t>
-  </si>
-  <si>
-    <t>03/17/2014 (Feb)</t>
-  </si>
-  <si>
-    <t>02/24/2014 (Jan)</t>
-  </si>
-  <si>
-    <t>01/16/2014 (Dec)</t>
-  </si>
-  <si>
-    <t>12/17/2013 (Nov)</t>
-  </si>
-  <si>
-    <t>11/15/2013 (Oct)</t>
-  </si>
-  <si>
-    <t>10/16/2013 (Sep)</t>
-  </si>
-  <si>
-    <t>09/16/2013 (Aug)</t>
-  </si>
-  <si>
-    <t>08/16/2013 (Jul)</t>
-  </si>
-  <si>
-    <t>07/16/2013 (Jun)</t>
-  </si>
-  <si>
-    <t>06/14/2013 (May)</t>
-  </si>
-  <si>
-    <t>05/16/2013 (Apr)</t>
-  </si>
-  <si>
-    <t>04/16/2013 (Mar)</t>
-  </si>
-  <si>
-    <t>03/15/2013 (Feb)</t>
-  </si>
-  <si>
-    <t>02/28/2013 (Jan)</t>
-  </si>
-  <si>
-    <t>01/16/2013 (Dec)</t>
-  </si>
-  <si>
-    <t>12/14/2012 (Nov)</t>
-  </si>
-  <si>
-    <t>11/15/2012 (Oct)</t>
-  </si>
-  <si>
-    <t>10/16/2012 (Sep)</t>
-  </si>
-  <si>
-    <t>09/14/2012 (Aug)</t>
-  </si>
-  <si>
-    <t>08/16/2012 (Jul)</t>
-  </si>
-  <si>
-    <t>07/16/2012 (Jun)</t>
-  </si>
-  <si>
-    <t>06/14/2012 (May)</t>
-  </si>
-  <si>
-    <t>05/16/2012 (Apr)</t>
-  </si>
-  <si>
-    <t>04/17/2012 (Mar)</t>
-  </si>
-  <si>
-    <t>03/14/2012 (Feb)</t>
-  </si>
-  <si>
-    <t>02/29/2012 (Jan)</t>
-  </si>
-  <si>
-    <t>01/17/2012 (Dec)</t>
-  </si>
-  <si>
-    <t>12/15/2011 (Nov)</t>
-  </si>
-  <si>
-    <t>11/16/2011 (Oct)</t>
-  </si>
-  <si>
-    <t>10/14/2011 (Sep)</t>
-  </si>
-  <si>
-    <t>09/15/2011 (Aug)</t>
-  </si>
-  <si>
-    <t>08/17/2011 (Jul)</t>
-  </si>
-  <si>
-    <t>07/14/2011 (Jun)</t>
-  </si>
-  <si>
-    <t>06/16/2011 (May)</t>
-  </si>
-  <si>
-    <t>05/16/2011 (Apr)</t>
-  </si>
-  <si>
-    <t>04/15/2011 (Mar)</t>
-  </si>
-  <si>
-    <t>03/16/2011 (Feb)</t>
-  </si>
-  <si>
-    <t>02/28/2011 (Jan)</t>
-  </si>
-  <si>
-    <t>01/14/2011 (Dec)</t>
-  </si>
-  <si>
-    <t>12/16/2010 (Nov)</t>
-  </si>
-  <si>
-    <t>11/16/2010 (Oct)</t>
-  </si>
-  <si>
-    <t>10/15/2010 (Sep)</t>
-  </si>
-  <si>
-    <t>09/15/2010 (Aug)</t>
-  </si>
-  <si>
-    <t>08/16/2010 (Jul)</t>
-  </si>
-  <si>
-    <t>07/14/2010 (Jun)</t>
-  </si>
-  <si>
-    <t>06/16/2010 (May)</t>
-  </si>
-  <si>
-    <t>05/18/2010 (Apr)</t>
-  </si>
-  <si>
-    <t>04/16/2010 (Mar)</t>
-  </si>
-  <si>
-    <t>03/16/2010 (Feb)</t>
-  </si>
-  <si>
-    <t>02/26/2010 (Jan)</t>
-  </si>
-  <si>
-    <t>01/15/2010 (Dec)</t>
-  </si>
-  <si>
-    <t>12/16/2009 (Nov)</t>
-  </si>
-  <si>
-    <t>11/16/2009 (Oct)</t>
-  </si>
-  <si>
-    <t>10/15/2009 (Sep)</t>
-  </si>
-  <si>
-    <t>09/16/2009 (Aug)</t>
-  </si>
-  <si>
-    <t>08/14/2009 (Jul)</t>
-  </si>
-  <si>
-    <t>07/15/2009 (Jun)</t>
-  </si>
-  <si>
-    <t>06/16/2009 (May)</t>
-  </si>
-  <si>
-    <t>05/15/2009 (Apr)</t>
-  </si>
-  <si>
-    <t>04/16/2009 (Mar)</t>
-  </si>
-  <si>
-    <t>03/16/2009 (Feb)</t>
-  </si>
-  <si>
-    <t>02/27/2009 (Jan)</t>
-  </si>
-  <si>
-    <t>01/15/2009 (Dec)</t>
-  </si>
-  <si>
-    <t>12/17/2008 (Nov)</t>
-  </si>
-  <si>
-    <t>11/14/2008 (Oct)</t>
-  </si>
-  <si>
-    <t>10/15/2008 (Sep)</t>
-  </si>
-  <si>
-    <t>09/16/2008 (Aug)</t>
-  </si>
-  <si>
-    <t>08/14/2008 (Jul)</t>
-  </si>
-  <si>
-    <t>07/16/2008 (Jun)</t>
-  </si>
-  <si>
-    <t>06/16/2008 (May)</t>
-  </si>
-  <si>
-    <t>05/15/2008 (Apr)</t>
-  </si>
-  <si>
-    <t>04/16/2008 (Mar)</t>
-  </si>
-  <si>
-    <t>03/14/2008 (Feb)</t>
-  </si>
-  <si>
-    <t>02/29/2008 (Jan)</t>
-  </si>
-  <si>
-    <t>01/16/2008 (Dec)</t>
-  </si>
-  <si>
-    <t>12/14/2007 (Nov)</t>
-  </si>
-  <si>
-    <t>11/15/2007 (Oct)</t>
-  </si>
-  <si>
-    <t>10/16/2007 (Sep)</t>
-  </si>
-  <si>
-    <t>09/14/2007 (Aug)</t>
-  </si>
-  <si>
-    <t>08/16/2007 (Jul)</t>
-  </si>
-  <si>
-    <t>07/16/2007 (Jun)</t>
-  </si>
-  <si>
-    <t>06/14/2007 (May)</t>
-  </si>
-  <si>
-    <t>05/16/2007 (Apr)</t>
-  </si>
-  <si>
-    <t>04/16/2007 (Mar)</t>
-  </si>
-  <si>
-    <t>03/15/2007 (Feb)</t>
-  </si>
-  <si>
-    <t>02/28/2007 (Jan)</t>
-  </si>
-  <si>
     <t>Actual</t>
   </si>
   <si>
@@ -605,13 +128,490 @@
   </si>
   <si>
     <t>¿negativo?</t>
+  </si>
+  <si>
+    <t>04/17/2020 09:00:00</t>
+  </si>
+  <si>
+    <t>03/18/2020 09:00:00</t>
+  </si>
+  <si>
+    <t>02/21/2020 09:00:00</t>
+  </si>
+  <si>
+    <t>01/17/2020 09:00:00</t>
+  </si>
+  <si>
+    <t>12/18/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>10/16/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>05/17/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>04/17/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>03/15/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>12/17/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>11/16/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>10/17/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>09/17/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>08/17/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>07/18/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>04/17/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>04/17/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>11/15/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>09/18/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>08/19/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>07/17/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>06/18/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>02/22/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>01/17/2019 09:00:00</t>
+  </si>
+  <si>
+    <t>06/15/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>05/16/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>04/18/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>03/16/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>02/23/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>01/17/2018 09:00:00</t>
+  </si>
+  <si>
+    <t>12/18/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>11/16/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>10/17/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>09/18/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>08/17/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>07/17/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>06/16/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>05/17/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>04/19/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>03/16/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>02/22/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>01/18/2017 09:00:00</t>
+  </si>
+  <si>
+    <t>12/16/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>11/17/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>10/17/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>09/15/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>08/18/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>07/15/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>06/16/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>05/18/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>04/14/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>03/17/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>02/25/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>01/19/2016 09:00:00</t>
+  </si>
+  <si>
+    <t>12/16/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>11/16/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>10/16/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>09/16/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>08/14/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>07/16/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>06/17/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>05/19/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>03/17/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>02/24/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>01/16/2015 09:00:00</t>
+  </si>
+  <si>
+    <t>12/17/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>11/14/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>10/16/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>09/17/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>08/14/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>07/17/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>06/16/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>05/15/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>04/16/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>03/17/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>02/24/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>01/16/2014 09:00:00</t>
+  </si>
+  <si>
+    <t>12/17/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>11/15/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>10/16/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>09/16/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>08/16/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>07/16/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>06/14/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>05/16/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>04/16/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>03/15/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>02/28/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>01/16/2013 09:00:00</t>
+  </si>
+  <si>
+    <t>12/14/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>11/15/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>10/16/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>09/14/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>08/16/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>07/16/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>06/14/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>05/16/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>03/14/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>02/29/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>01/17/2012 09:00:00</t>
+  </si>
+  <si>
+    <t>12/15/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>11/16/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>10/14/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>09/14/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>08/15/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>07/17/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>06/14/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>06/16/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>05/16/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>04/15/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>03/16/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>02/14/2011 09:00:00</t>
+  </si>
+  <si>
+    <t>01/14/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>11/16/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>10/15/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>09/15/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>08/16/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>07/14/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>06/16/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>05/18/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>04/16/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>03/16/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>02/26/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>01/15/2010 09:00:00</t>
+  </si>
+  <si>
+    <t>12/16/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>11/16/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>10/15/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>04/16/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>08/14/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>09/16/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>07/15/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>06/16/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>05/15/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>03/15/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>02/27/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>01/15/2009 09:00:00</t>
+  </si>
+  <si>
+    <t>12/17/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>11/14/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>10/15/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>09/16/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>08/14/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>07/16/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>06/16/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>05/15/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>04/16/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>03/14/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>02/29/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>01/16/2008 09:00:00</t>
+  </si>
+  <si>
+    <t>12/14/2007 09:00:00</t>
+  </si>
+  <si>
+    <t>11/15/2007 09:00:00</t>
+  </si>
+  <si>
+    <t>10/16/2007 09:00:00</t>
+  </si>
+  <si>
+    <t>09/14/2007 09:00:00</t>
+  </si>
+  <si>
+    <t>08/16/2007 09:00:00</t>
+  </si>
+  <si>
+    <t>07/16/2007 09:00:00</t>
+  </si>
+  <si>
+    <t>06/14/2007 09:00:00</t>
+  </si>
+  <si>
+    <t>05/16/2007 09:00:00</t>
+  </si>
+  <si>
+    <t>04/16/2007 09:00:00</t>
+  </si>
+  <si>
+    <t>03/15/2007 09:00:00</t>
+  </si>
+  <si>
+    <t>02/28/2007 09:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,12 +622,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF49494F"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1B1C23"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -708,13 +702,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF24292E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -728,30 +740,30 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -763,35 +775,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2077,35 +2089,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04AE2B0B-1D69-46F2-8B2F-B4F5CB2C831F}">
   <dimension ref="A1:E296"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>160</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>163</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>161</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>162</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
+      <c r="A2" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="B2" s="3">
         <v>0.5</v>
@@ -2121,8 +2134,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>1</v>
+      <c r="A3" s="22" t="s">
+        <v>33</v>
       </c>
       <c r="B3" s="3">
         <v>0.2</v>
@@ -2138,8 +2151,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>2</v>
+      <c r="A4" s="22" t="s">
+        <v>34</v>
       </c>
       <c r="B4" s="3">
         <v>-1</v>
@@ -2155,8 +2168,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>3</v>
+      <c r="A5" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="B5" s="3">
         <v>0.3</v>
@@ -2172,8 +2185,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>4</v>
+      <c r="A6" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="B6" s="3">
         <v>-0.3</v>
@@ -2189,10 +2202,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="18">
+      <c r="A7" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="17">
         <v>0.1</v>
       </c>
       <c r="C7" s="3">
@@ -2206,8 +2219,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>6</v>
+      <c r="A8" s="22" t="s">
+        <v>37</v>
       </c>
       <c r="B8" s="3">
         <v>0.2</v>
@@ -2223,10 +2236,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="18">
+      <c r="A9" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="17">
         <v>0.1</v>
       </c>
       <c r="C9" s="3">
@@ -2240,10 +2253,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="18">
+      <c r="A10" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="17">
         <v>-0.5</v>
       </c>
       <c r="C10" s="3">
@@ -2257,10 +2270,10 @@
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="19">
+      <c r="A11" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="18">
         <v>0.2</v>
       </c>
       <c r="C11" s="3">
@@ -2274,10 +2287,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="18">
+      <c r="A12" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="17">
         <v>0.1</v>
       </c>
       <c r="C12" s="3">
@@ -2291,8 +2304,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>11</v>
+      <c r="A13" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="B13" s="3">
         <v>0.7</v>
@@ -2308,8 +2321,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>12</v>
+      <c r="A14" s="22" t="s">
+        <v>39</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
@@ -2325,8 +2338,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>13</v>
+      <c r="A15" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="B15" s="3">
         <v>0.3</v>
@@ -2342,10 +2355,10 @@
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="19">
+      <c r="A16" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="18">
         <v>-1</v>
       </c>
       <c r="C16" s="3">
@@ -2357,8 +2370,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>15</v>
+      <c r="A17" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -2372,8 +2385,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>16</v>
+      <c r="A18" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="B18" s="3">
         <v>-0.2</v>
@@ -2389,8 +2402,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>17</v>
+      <c r="A19" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="B19" s="3">
         <v>0.2</v>
@@ -2406,8 +2419,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>18</v>
+      <c r="A20" s="22" t="s">
+        <v>43</v>
       </c>
       <c r="B20" s="3">
         <v>0.5</v>
@@ -2423,8 +2436,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>19</v>
+      <c r="A21" s="22" t="s">
+        <v>44</v>
       </c>
       <c r="B21" s="3">
         <v>0.2</v>
@@ -2440,8 +2453,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>20</v>
+      <c r="A22" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="B22" s="3">
         <v>-0.3</v>
@@ -2457,8 +2470,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>21</v>
+      <c r="A23" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="B23" s="3">
         <v>0.1</v>
@@ -2474,8 +2487,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
-        <v>22</v>
+      <c r="A24" s="22" t="s">
+        <v>56</v>
       </c>
       <c r="B24" s="3">
         <v>0.5</v>
@@ -2491,8 +2504,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>23</v>
+      <c r="A25" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="B25" s="3">
         <v>0.3</v>
@@ -2508,8 +2521,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>24</v>
+      <c r="A26" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="B26" s="3">
         <v>1</v>
@@ -2525,8 +2538,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>25</v>
+      <c r="A27" s="22" t="s">
+        <v>59</v>
       </c>
       <c r="B27" s="3">
         <v>0.2</v>
@@ -2542,8 +2555,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>26</v>
+      <c r="A28" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="B28" s="3">
         <v>-0.9</v>
@@ -2559,8 +2572,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
-        <v>27</v>
+      <c r="A29" s="22" t="s">
+        <v>61</v>
       </c>
       <c r="B29" s="3">
         <v>0.4</v>
@@ -2576,8 +2589,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>28</v>
+      <c r="A30" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="B30" s="3">
         <v>0.1</v>
@@ -2593,8 +2606,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>29</v>
+      <c r="A31" s="22" t="s">
+        <v>63</v>
       </c>
       <c r="B31" s="3">
         <v>0.1</v>
@@ -2610,8 +2623,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
-        <v>30</v>
+      <c r="A32" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="B32" s="3">
         <v>0.4</v>
@@ -2627,8 +2640,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
-        <v>31</v>
+      <c r="A33" s="22" t="s">
+        <v>65</v>
       </c>
       <c r="B33" s="3">
         <v>0.3</v>
@@ -2644,8 +2657,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>32</v>
+      <c r="A34" s="22" t="s">
+        <v>66</v>
       </c>
       <c r="B34" s="3">
         <v>-0.5</v>
@@ -2661,8 +2674,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>33</v>
+      <c r="A35" s="22" t="s">
+        <v>67</v>
       </c>
       <c r="B35" s="3">
         <v>0</v>
@@ -2678,8 +2691,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>34</v>
+      <c r="A36" s="22" t="s">
+        <v>68</v>
       </c>
       <c r="B36" s="3">
         <v>-0.1</v>
@@ -2695,8 +2708,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
-        <v>35</v>
+      <c r="A37" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="B37" s="3">
         <v>0.4</v>
@@ -2712,8 +2725,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>36</v>
+      <c r="A38" s="22" t="s">
+        <v>70</v>
       </c>
       <c r="B38" s="3">
         <v>0.8</v>
@@ -2729,8 +2742,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
-        <v>37</v>
+      <c r="A39" s="22" t="s">
+        <v>71</v>
       </c>
       <c r="B39" s="3">
         <v>0.4</v>
@@ -2746,8 +2759,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
-        <v>38</v>
+      <c r="A40" s="22" t="s">
+        <v>72</v>
       </c>
       <c r="B40" s="3">
         <v>-0.8</v>
@@ -2763,8 +2776,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
-        <v>39</v>
+      <c r="A41" s="22" t="s">
+        <v>73</v>
       </c>
       <c r="B41" s="3">
         <v>0.5</v>
@@ -2780,8 +2793,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
-        <v>40</v>
+      <c r="A42" s="22" t="s">
+        <v>74</v>
       </c>
       <c r="B42" s="3">
         <v>-0.1</v>
@@ -2797,10 +2810,10 @@
       </c>
     </row>
     <row r="43" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" s="18">
+      <c r="A43" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="17">
         <v>0.2</v>
       </c>
       <c r="C43" s="3">
@@ -2814,8 +2827,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>42</v>
+      <c r="A44" s="22" t="s">
+        <v>76</v>
       </c>
       <c r="B44" s="3">
         <v>0.4</v>
@@ -2831,8 +2844,8 @@
       </c>
     </row>
     <row r="45" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
-        <v>43</v>
+      <c r="A45" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="B45" s="3">
         <v>0.1</v>
@@ -2848,10 +2861,10 @@
       </c>
     </row>
     <row r="46" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="18">
+      <c r="A46" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="17">
         <v>-0.6</v>
       </c>
       <c r="C46" s="3">
@@ -2865,8 +2878,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
-        <v>45</v>
+      <c r="A47" s="22" t="s">
+        <v>79</v>
       </c>
       <c r="B47" s="3">
         <v>0.2</v>
@@ -2882,10 +2895,10 @@
       </c>
     </row>
     <row r="48" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="19">
+      <c r="A48" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="18">
         <v>0.4</v>
       </c>
       <c r="C48" s="3">
@@ -2899,8 +2912,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
-        <v>47</v>
+      <c r="A49" s="22" t="s">
+        <v>81</v>
       </c>
       <c r="B49" s="3">
         <v>0</v>
@@ -2916,8 +2929,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
-        <v>48</v>
+      <c r="A50" s="22" t="s">
+        <v>82</v>
       </c>
       <c r="B50" s="3">
         <v>1.2</v>
@@ -2933,10 +2946,10 @@
       </c>
     </row>
     <row r="51" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="19">
+      <c r="A51" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="18">
         <v>0.2</v>
       </c>
       <c r="C51" s="3">
@@ -2950,8 +2963,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
-        <v>50</v>
+      <c r="A52" s="22" t="s">
+        <v>84</v>
       </c>
       <c r="B52" s="3">
         <v>-1.4</v>
@@ -2963,8 +2976,8 @@
       <c r="E52" s="3"/>
     </row>
     <row r="53" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
-        <v>51</v>
+      <c r="A53" s="22" t="s">
+        <v>85</v>
       </c>
       <c r="B53" s="3">
         <v>0</v>
@@ -2980,8 +2993,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
-        <v>52</v>
+      <c r="A54" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="B54" s="3">
         <v>-0.1</v>
@@ -2997,8 +3010,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
-        <v>53</v>
+      <c r="A55" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="B55" s="3">
         <v>0.1</v>
@@ -3014,8 +3027,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>54</v>
+      <c r="A56" s="22" t="s">
+        <v>88</v>
       </c>
       <c r="B56" s="3">
         <v>0.2</v>
@@ -3031,8 +3044,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
-        <v>55</v>
+      <c r="A57" s="22" t="s">
+        <v>89</v>
       </c>
       <c r="B57" s="3">
         <v>0</v>
@@ -3048,8 +3061,8 @@
       </c>
     </row>
     <row r="58" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
-        <v>56</v>
+      <c r="A58" s="22" t="s">
+        <v>90</v>
       </c>
       <c r="B58" s="3">
         <v>-0.6</v>
@@ -3065,8 +3078,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
-        <v>57</v>
+      <c r="A59" s="22" t="s">
+        <v>91</v>
       </c>
       <c r="B59" s="3">
         <v>0</v>
@@ -3082,8 +3095,8 @@
       </c>
     </row>
     <row r="60" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
-        <v>58</v>
+      <c r="A60" s="22" t="s">
+        <v>92</v>
       </c>
       <c r="B60" s="3">
         <v>0.2</v>
@@ -3099,8 +3112,8 @@
       </c>
     </row>
     <row r="61" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
-        <v>59</v>
+      <c r="A61" s="22" t="s">
+        <v>93</v>
       </c>
       <c r="B61" s="3">
         <v>0.2</v>
@@ -3116,8 +3129,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
-        <v>60</v>
+      <c r="A62" s="22" t="s">
+        <v>47</v>
       </c>
       <c r="B62" s="3">
         <v>1.1000000000000001</v>
@@ -3133,8 +3146,8 @@
       </c>
     </row>
     <row r="63" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
-        <v>61</v>
+      <c r="A63" s="22" t="s">
+        <v>94</v>
       </c>
       <c r="B63" s="3">
         <v>0.6</v>
@@ -3150,8 +3163,8 @@
       </c>
     </row>
     <row r="64" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
-        <v>62</v>
+      <c r="A64" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="B64" s="3">
         <v>-1.6</v>
@@ -3167,8 +3180,8 @@
       </c>
     </row>
     <row r="65" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="17" t="s">
-        <v>63</v>
+      <c r="A65" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="B65" s="3">
         <v>-0.1</v>
@@ -3184,8 +3197,8 @@
       </c>
     </row>
     <row r="66" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
-        <v>64</v>
+      <c r="A66" s="22" t="s">
+        <v>97</v>
       </c>
       <c r="B66" s="3">
         <v>-0.2</v>
@@ -3201,8 +3214,8 @@
       </c>
     </row>
     <row r="67" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="17" t="s">
-        <v>65</v>
+      <c r="A67" s="22" t="s">
+        <v>98</v>
       </c>
       <c r="B67" s="3">
         <v>0</v>
@@ -3218,8 +3231,8 @@
       </c>
     </row>
     <row r="68" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="17" t="s">
-        <v>66</v>
+      <c r="A68" s="22" t="s">
+        <v>99</v>
       </c>
       <c r="B68" s="3">
         <v>0.4</v>
@@ -3235,8 +3248,8 @@
       </c>
     </row>
     <row r="69" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
-        <v>67</v>
+      <c r="A69" s="22" t="s">
+        <v>100</v>
       </c>
       <c r="B69" s="3">
         <v>0.1</v>
@@ -3252,10 +3265,10 @@
       </c>
     </row>
     <row r="70" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B70" s="18">
+      <c r="A70" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B70" s="17">
         <v>-0.7</v>
       </c>
       <c r="C70" s="3">
@@ -3269,8 +3282,8 @@
       </c>
     </row>
     <row r="71" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
-        <v>69</v>
+      <c r="A71" s="22" t="s">
+        <v>102</v>
       </c>
       <c r="B71" s="3">
         <v>0.1</v>
@@ -3286,8 +3299,8 @@
       </c>
     </row>
     <row r="72" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
-        <v>70</v>
+      <c r="A72" s="22" t="s">
+        <v>103</v>
       </c>
       <c r="B72" s="3">
         <v>-0.1</v>
@@ -3303,8 +3316,8 @@
       </c>
     </row>
     <row r="73" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
-        <v>71</v>
+      <c r="A73" s="22" t="s">
+        <v>104</v>
       </c>
       <c r="B73" s="3">
         <v>0.2</v>
@@ -3320,10 +3333,10 @@
       </c>
     </row>
     <row r="74" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B74" s="18">
+      <c r="A74" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B74" s="17">
         <v>0.9</v>
       </c>
       <c r="C74" s="3">
@@ -3337,10 +3350,10 @@
       </c>
     </row>
     <row r="75" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B75" s="18">
+      <c r="A75" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B75" s="17">
         <v>0.3</v>
       </c>
       <c r="C75" s="3">
@@ -3354,8 +3367,8 @@
       </c>
     </row>
     <row r="76" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
-        <v>74</v>
+      <c r="A76" s="22" t="s">
+        <v>107</v>
       </c>
       <c r="B76" s="3">
         <v>-1.1000000000000001</v>
@@ -3371,8 +3384,8 @@
       </c>
     </row>
     <row r="77" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
-        <v>75</v>
+      <c r="A77" s="22" t="s">
+        <v>108</v>
       </c>
       <c r="B77" s="3">
         <v>0.3</v>
@@ -3388,8 +3401,8 @@
       </c>
     </row>
     <row r="78" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
-        <v>76</v>
+      <c r="A78" s="22" t="s">
+        <v>109</v>
       </c>
       <c r="B78" s="3">
         <v>-0.1</v>
@@ -3405,8 +3418,8 @@
       </c>
     </row>
     <row r="79" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
-        <v>77</v>
+      <c r="A79" s="22" t="s">
+        <v>110</v>
       </c>
       <c r="B79" s="3">
         <v>-0.1</v>
@@ -3422,8 +3435,8 @@
       </c>
     </row>
     <row r="80" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
-        <v>78</v>
+      <c r="A80" s="22" t="s">
+        <v>111</v>
       </c>
       <c r="B80" s="3">
         <v>0.5</v>
@@ -3439,8 +3452,8 @@
       </c>
     </row>
     <row r="81" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
-        <v>79</v>
+      <c r="A81" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="B81" s="3">
         <v>0.1</v>
@@ -3456,8 +3469,8 @@
       </c>
     </row>
     <row r="82" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
-        <v>80</v>
+      <c r="A82" s="22" t="s">
+        <v>113</v>
       </c>
       <c r="B82" s="3">
         <v>-0.5</v>
@@ -3473,8 +3486,8 @@
       </c>
     </row>
     <row r="83" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
-        <v>81</v>
+      <c r="A83" s="22" t="s">
+        <v>114</v>
       </c>
       <c r="B83" s="3">
         <v>0.1</v>
@@ -3490,8 +3503,8 @@
       </c>
     </row>
     <row r="84" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="17" t="s">
-        <v>82</v>
+      <c r="A84" s="22" t="s">
+        <v>115</v>
       </c>
       <c r="B84" s="3">
         <v>0.1</v>
@@ -3507,8 +3520,8 @@
       </c>
     </row>
     <row r="85" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="17" t="s">
-        <v>83</v>
+      <c r="A85" s="22" t="s">
+        <v>116</v>
       </c>
       <c r="B85" s="3">
         <v>-0.1</v>
@@ -3524,8 +3537,8 @@
       </c>
     </row>
     <row r="86" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="17" t="s">
-        <v>84</v>
+      <c r="A86" s="22" t="s">
+        <v>117</v>
       </c>
       <c r="B86" s="3">
         <v>1.2</v>
@@ -3541,8 +3554,8 @@
       </c>
     </row>
     <row r="87" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="17" t="s">
-        <v>85</v>
+      <c r="A87" s="22" t="s">
+        <v>118</v>
       </c>
       <c r="B87" s="3">
         <v>0.4</v>
@@ -3558,8 +3571,8 @@
       </c>
     </row>
     <row r="88" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="17" t="s">
-        <v>86</v>
+      <c r="A88" s="22" t="s">
+        <v>119</v>
       </c>
       <c r="B88" s="3">
         <v>-1</v>
@@ -3575,10 +3588,10 @@
       </c>
     </row>
     <row r="89" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B89" s="19">
+      <c r="A89" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B89" s="18">
         <v>0.4</v>
       </c>
       <c r="C89" s="3">
@@ -3592,8 +3605,8 @@
       </c>
     </row>
     <row r="90" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
-        <v>88</v>
+      <c r="A90" s="22" t="s">
+        <v>121</v>
       </c>
       <c r="B90" s="3">
         <v>-0.2</v>
@@ -3609,8 +3622,8 @@
       </c>
     </row>
     <row r="91" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="17" t="s">
-        <v>89</v>
+      <c r="A91" s="22" t="s">
+        <v>122</v>
       </c>
       <c r="B91" s="3">
         <v>0.2</v>
@@ -3626,10 +3639,10 @@
       </c>
     </row>
     <row r="92" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B92" s="18">
+      <c r="A92" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B92" s="17">
         <v>0.7</v>
       </c>
       <c r="C92" s="3">
@@ -3643,8 +3656,8 @@
       </c>
     </row>
     <row r="93" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="17" t="s">
-        <v>91</v>
+      <c r="A93" s="22" t="s">
+        <v>124</v>
       </c>
       <c r="B93" s="3">
         <v>0.4</v>
@@ -3660,8 +3673,8 @@
       </c>
     </row>
     <row r="94" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
-        <v>92</v>
+      <c r="A94" s="22" t="s">
+        <v>125</v>
       </c>
       <c r="B94" s="3">
         <v>-0.5</v>
@@ -3677,10 +3690,10 @@
       </c>
     </row>
     <row r="95" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="B95" s="18">
+      <c r="A95" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B95" s="17">
         <v>-0.1</v>
       </c>
       <c r="C95" s="3">
@@ -3694,10 +3707,10 @@
       </c>
     </row>
     <row r="96" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B96" s="19">
+      <c r="A96" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B96" s="18">
         <v>-0.1</v>
       </c>
       <c r="C96" s="3">
@@ -3711,8 +3724,8 @@
       </c>
     </row>
     <row r="97" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="17" t="s">
-        <v>95</v>
+      <c r="A97" s="22" t="s">
+        <v>128</v>
       </c>
       <c r="B97" s="3">
         <v>0.5</v>
@@ -3728,10 +3741,10 @@
       </c>
     </row>
     <row r="98" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B98" s="19">
+      <c r="A98" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B98" s="18">
         <v>1.3</v>
       </c>
       <c r="C98" s="3">
@@ -3745,8 +3758,8 @@
       </c>
     </row>
     <row r="99" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="17" t="s">
-        <v>97</v>
+      <c r="A99" s="22" t="s">
+        <v>129</v>
       </c>
       <c r="B99" s="3">
         <v>0.5</v>
@@ -3762,8 +3775,8 @@
       </c>
     </row>
     <row r="100" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="17" t="s">
-        <v>98</v>
+      <c r="A100" s="22" t="s">
+        <v>130</v>
       </c>
       <c r="B100" s="3">
         <v>-0.8</v>
@@ -3779,10 +3792,10 @@
       </c>
     </row>
     <row r="101" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B101" s="18">
+      <c r="A101" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B101" s="17">
         <v>0.3</v>
       </c>
       <c r="C101" s="3">
@@ -3796,8 +3809,8 @@
       </c>
     </row>
     <row r="102" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="17" t="s">
-        <v>100</v>
+      <c r="A102" s="22" t="s">
+        <v>132</v>
       </c>
       <c r="B102" s="3">
         <v>0.1</v>
@@ -3813,8 +3826,8 @@
       </c>
     </row>
     <row r="103" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="17" t="s">
-        <v>101</v>
+      <c r="A103" s="22" t="s">
+        <v>133</v>
       </c>
       <c r="B103" s="3">
         <v>0.3</v>
@@ -3830,8 +3843,8 @@
       </c>
     </row>
     <row r="104" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="17" t="s">
-        <v>102</v>
+      <c r="A104" s="22" t="s">
+        <v>134</v>
       </c>
       <c r="B104" s="3">
         <v>0.8</v>
@@ -3843,8 +3856,8 @@
       <c r="E104" s="3"/>
     </row>
     <row r="105" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="17" t="s">
-        <v>103</v>
+      <c r="A105" s="22" t="s">
+        <v>135</v>
       </c>
       <c r="B105" s="3">
         <v>0.2</v>
@@ -3860,8 +3873,8 @@
       </c>
     </row>
     <row r="106" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="17" t="s">
-        <v>104</v>
+      <c r="A106" s="22" t="s">
+        <v>136</v>
       </c>
       <c r="B106" s="3">
         <v>-0.6</v>
@@ -3877,8 +3890,8 @@
       </c>
     </row>
     <row r="107" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="17" t="s">
-        <v>105</v>
+      <c r="A107" s="22" t="s">
+        <v>137</v>
       </c>
       <c r="B107" s="3">
         <v>0</v>
@@ -3894,8 +3907,8 @@
       </c>
     </row>
     <row r="108" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="17" t="s">
-        <v>106</v>
+      <c r="A108" s="22" t="s">
+        <v>138</v>
       </c>
       <c r="B108" s="3">
         <v>0</v>
@@ -3911,8 +3924,8 @@
       </c>
     </row>
     <row r="109" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="17" t="s">
-        <v>107</v>
+      <c r="A109" s="22" t="s">
+        <v>139</v>
       </c>
       <c r="B109" s="3">
         <v>0.6</v>
@@ -3928,10 +3941,10 @@
       </c>
     </row>
     <row r="110" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B110" s="19">
+      <c r="A110" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B110" s="18">
         <v>1.4</v>
       </c>
       <c r="C110" s="3">
@@ -3945,8 +3958,8 @@
       </c>
     </row>
     <row r="111" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="17" t="s">
-        <v>109</v>
+      <c r="A111" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="B111" s="3">
         <v>0.4</v>
@@ -3962,10 +3975,10 @@
       </c>
     </row>
     <row r="112" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="B112" s="18">
+      <c r="A112" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="B112" s="17">
         <v>-0.7</v>
       </c>
       <c r="C112" s="3">
@@ -3979,8 +3992,8 @@
       </c>
     </row>
     <row r="113" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="17" t="s">
-        <v>111</v>
+      <c r="A113" s="22" t="s">
+        <v>143</v>
       </c>
       <c r="B113" s="3">
         <v>0.6</v>
@@ -3996,8 +4009,8 @@
       </c>
     </row>
     <row r="114" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="17" t="s">
-        <v>112</v>
+      <c r="A114" s="22" t="s">
+        <v>144</v>
       </c>
       <c r="B114" s="3">
         <v>0.1</v>
@@ -4011,10 +4024,10 @@
       </c>
     </row>
     <row r="115" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B115" s="19">
+      <c r="A115" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B115" s="18">
         <v>0.4</v>
       </c>
       <c r="C115" s="3">
@@ -4026,8 +4039,8 @@
       </c>
     </row>
     <row r="116" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="17" t="s">
-        <v>114</v>
+      <c r="A116" s="22" t="s">
+        <v>146</v>
       </c>
       <c r="B116" s="3">
         <v>0.2</v>
@@ -4041,8 +4054,8 @@
       </c>
     </row>
     <row r="117" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="17" t="s">
-        <v>115</v>
+      <c r="A117" s="22" t="s">
+        <v>147</v>
       </c>
       <c r="B117" s="3">
         <v>0.2</v>
@@ -4056,10 +4069,10 @@
       </c>
     </row>
     <row r="118" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B118" s="19">
+      <c r="A118" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="B118" s="18">
         <v>-0.3</v>
       </c>
       <c r="C118" s="3">
@@ -4071,8 +4084,8 @@
       </c>
     </row>
     <row r="119" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="17" t="s">
-        <v>117</v>
+      <c r="A119" s="22" t="s">
+        <v>149</v>
       </c>
       <c r="B119" s="3">
         <v>0</v>
@@ -4086,8 +4099,8 @@
       </c>
     </row>
     <row r="120" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="17" t="s">
-        <v>118</v>
+      <c r="A120" s="22" t="s">
+        <v>150</v>
       </c>
       <c r="B120" s="3">
         <v>0.1</v>
@@ -4101,10 +4114,10 @@
       </c>
     </row>
     <row r="121" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B121" s="19">
+      <c r="A121" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="B121" s="18">
         <v>0.5</v>
       </c>
       <c r="C121" s="3">
@@ -4116,8 +4129,8 @@
       </c>
     </row>
     <row r="122" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="17" t="s">
-        <v>120</v>
+      <c r="A122" s="22" t="s">
+        <v>152</v>
       </c>
       <c r="B122" s="3">
         <v>0.9</v>
@@ -4131,8 +4144,8 @@
       </c>
     </row>
     <row r="123" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="17" t="s">
-        <v>121</v>
+      <c r="A123" s="22" t="s">
+        <v>153</v>
       </c>
       <c r="B123" s="3">
         <v>0.3</v>
@@ -4146,10 +4159,10 @@
       </c>
     </row>
     <row r="124" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="B124" s="18">
+      <c r="A124" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="B124" s="17">
         <v>-0.8</v>
       </c>
       <c r="C124" s="3">
@@ -4161,8 +4174,8 @@
       </c>
     </row>
     <row r="125" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="17" t="s">
-        <v>123</v>
+      <c r="A125" s="22" t="s">
+        <v>155</v>
       </c>
       <c r="B125" s="3">
         <v>0.3</v>
@@ -4176,10 +4189,10 @@
       </c>
     </row>
     <row r="126" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="B126" s="18">
+      <c r="A126" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B126" s="17">
         <v>0.1</v>
       </c>
       <c r="C126" s="3">
@@ -4191,10 +4204,10 @@
       </c>
     </row>
     <row r="127" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="B127" s="18">
+      <c r="A127" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B127" s="17">
         <v>0.2</v>
       </c>
       <c r="C127" s="3">
@@ -4206,10 +4219,10 @@
       </c>
     </row>
     <row r="128" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B128" s="18">
+      <c r="A128" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="B128" s="17">
         <v>0</v>
       </c>
       <c r="C128" s="3">
@@ -4221,8 +4234,8 @@
       </c>
     </row>
     <row r="129" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="17" t="s">
-        <v>127</v>
+      <c r="A129" s="22" t="s">
+        <v>161</v>
       </c>
       <c r="B129" s="3">
         <v>0.3</v>
@@ -4236,10 +4249,10 @@
       </c>
     </row>
     <row r="130" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B130" s="18">
+      <c r="A130" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B130" s="17">
         <v>-0.7</v>
       </c>
       <c r="C130" s="3">
@@ -4251,8 +4264,8 @@
       </c>
     </row>
     <row r="131" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="17" t="s">
-        <v>129</v>
+      <c r="A131" s="22" t="s">
+        <v>162</v>
       </c>
       <c r="B131" s="3">
         <v>0.2</v>
@@ -4266,10 +4279,10 @@
       </c>
     </row>
     <row r="132" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B132" s="19">
+      <c r="A132" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="B132" s="18">
         <v>0.1</v>
       </c>
       <c r="C132" s="3">
@@ -4281,8 +4294,8 @@
       </c>
     </row>
     <row r="133" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="17" t="s">
-        <v>131</v>
+      <c r="A133" s="22" t="s">
+        <v>164</v>
       </c>
       <c r="B133" s="3">
         <v>0.4</v>
@@ -4296,8 +4309,8 @@
       </c>
     </row>
     <row r="134" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="17" t="s">
-        <v>132</v>
+      <c r="A134" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B134" s="3">
         <v>0.4</v>
@@ -4311,8 +4324,8 @@
       </c>
     </row>
     <row r="135" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="17" t="s">
-        <v>133</v>
+      <c r="A135" s="22" t="s">
+        <v>165</v>
       </c>
       <c r="B135" s="3">
         <v>0.4</v>
@@ -4326,10 +4339,10 @@
       </c>
     </row>
     <row r="136" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B136" s="19">
+      <c r="A136" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="B136" s="18">
         <v>-0.8</v>
       </c>
       <c r="C136" s="3">
@@ -4341,8 +4354,8 @@
       </c>
     </row>
     <row r="137" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="17" t="s">
-        <v>135</v>
+      <c r="A137" s="22" t="s">
+        <v>167</v>
       </c>
       <c r="B137" s="3">
         <v>-0.1</v>
@@ -4356,8 +4369,8 @@
       </c>
     </row>
     <row r="138" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="17" t="s">
-        <v>136</v>
+      <c r="A138" s="22" t="s">
+        <v>168</v>
       </c>
       <c r="B138" s="3">
         <v>-0.5</v>
@@ -4371,10 +4384,10 @@
       </c>
     </row>
     <row r="139" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="B139" s="18">
+      <c r="A139" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B139" s="17">
         <v>0</v>
       </c>
       <c r="C139" s="3">
@@ -4386,10 +4399,10 @@
       </c>
     </row>
     <row r="140" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B140" s="19">
+      <c r="A140" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B140" s="18">
         <v>0.2</v>
       </c>
       <c r="C140" s="3">
@@ -4401,10 +4414,10 @@
       </c>
     </row>
     <row r="141" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="B141" s="19">
+      <c r="A141" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B141" s="18">
         <v>-0.1</v>
       </c>
       <c r="C141" s="3">
@@ -4416,10 +4429,10 @@
       </c>
     </row>
     <row r="142" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B142" s="18">
+      <c r="A142" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B142" s="17">
         <v>-0.2</v>
       </c>
       <c r="C142" s="3">
@@ -4431,8 +4444,8 @@
       </c>
     </row>
     <row r="143" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="17" t="s">
-        <v>141</v>
+      <c r="A143" s="22" t="s">
+        <v>173</v>
       </c>
       <c r="B143" s="3">
         <v>0.4</v>
@@ -4446,8 +4459,8 @@
       </c>
     </row>
     <row r="144" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="17" t="s">
-        <v>142</v>
+      <c r="A144" s="22" t="s">
+        <v>174</v>
       </c>
       <c r="B144" s="3">
         <v>0.6</v>
@@ -4461,8 +4474,8 @@
       </c>
     </row>
     <row r="145" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="17" t="s">
-        <v>143</v>
+      <c r="A145" s="22" t="s">
+        <v>175</v>
       </c>
       <c r="B145" s="3">
         <v>0.3</v>
@@ -4476,10 +4489,10 @@
       </c>
     </row>
     <row r="146" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B146" s="19">
+      <c r="A146" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B146" s="18">
         <v>1</v>
       </c>
       <c r="C146" s="3">
@@ -4491,8 +4504,8 @@
       </c>
     </row>
     <row r="147" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="17" t="s">
-        <v>145</v>
+      <c r="A147" s="22" t="s">
+        <v>177</v>
       </c>
       <c r="B147" s="3">
         <v>0.3</v>
@@ -4506,8 +4519,8 @@
       </c>
     </row>
     <row r="148" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="17" t="s">
-        <v>146</v>
+      <c r="A148" s="22" t="s">
+        <v>178</v>
       </c>
       <c r="B148" s="3">
         <v>-0.4</v>
@@ -4521,8 +4534,8 @@
       </c>
     </row>
     <row r="149" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="17" t="s">
-        <v>147</v>
+      <c r="A149" s="22" t="s">
+        <v>179</v>
       </c>
       <c r="B149" s="3">
         <v>0.4</v>
@@ -4536,8 +4549,8 @@
       </c>
     </row>
     <row r="150" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="17" t="s">
-        <v>148</v>
+      <c r="A150" s="22" t="s">
+        <v>180</v>
       </c>
       <c r="B150" s="3">
         <v>0.5</v>
@@ -4551,8 +4564,8 @@
       </c>
     </row>
     <row r="151" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="17" t="s">
-        <v>149</v>
+      <c r="A151" s="22" t="s">
+        <v>181</v>
       </c>
       <c r="B151" s="3">
         <v>0.5</v>
@@ -4566,8 +4579,8 @@
       </c>
     </row>
     <row r="152" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="17" t="s">
-        <v>150</v>
+      <c r="A152" s="22" t="s">
+        <v>182</v>
       </c>
       <c r="B152" s="3">
         <v>0.4</v>
@@ -4581,8 +4594,8 @@
       </c>
     </row>
     <row r="153" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="17" t="s">
-        <v>151</v>
+      <c r="A153" s="22" t="s">
+        <v>183</v>
       </c>
       <c r="B153" s="3">
         <v>0.1</v>
@@ -4596,8 +4609,8 @@
       </c>
     </row>
     <row r="154" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="17" t="s">
-        <v>152</v>
+      <c r="A154" s="22" t="s">
+        <v>184</v>
       </c>
       <c r="B154" s="3">
         <v>-0.2</v>
@@ -4611,8 +4624,8 @@
       </c>
     </row>
     <row r="155" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="17" t="s">
-        <v>153</v>
+      <c r="A155" s="22" t="s">
+        <v>185</v>
       </c>
       <c r="B155" s="3">
         <v>0.1</v>
@@ -4626,10 +4639,10 @@
       </c>
     </row>
     <row r="156" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="B156" s="18">
+      <c r="A156" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B156" s="17">
         <v>0.2</v>
       </c>
       <c r="C156" s="3">
@@ -4641,10 +4654,10 @@
       </c>
     </row>
     <row r="157" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="B157" s="19">
+      <c r="A157" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B157" s="18">
         <v>0.6</v>
       </c>
       <c r="C157" s="3">
@@ -4656,10 +4669,10 @@
       </c>
     </row>
     <row r="158" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="B158" s="19">
+      <c r="A158" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="B158" s="18">
         <v>0.7</v>
       </c>
       <c r="C158" s="3">
@@ -4671,8 +4684,8 @@
       </c>
     </row>
     <row r="159" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="17" t="s">
-        <v>157</v>
+      <c r="A159" s="22" t="s">
+        <v>189</v>
       </c>
       <c r="B159" s="3">
         <v>0.3</v>
@@ -4686,8 +4699,8 @@
       </c>
     </row>
     <row r="160" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="17" t="s">
-        <v>158</v>
+      <c r="A160" s="22" t="s">
+        <v>190</v>
       </c>
       <c r="B160" s="3">
         <v>-0.5</v>
@@ -5103,6 +5116,7 @@
     <row r="295" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="296" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5112,7 +5126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3584F10-7D3D-4957-9E2F-8A93B44E162A}">
   <dimension ref="A1:N141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -5124,18 +5138,18 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="20">
+        <v>5</v>
+      </c>
+      <c r="B1" s="19">
         <v>43882</v>
       </c>
       <c r="J1" t="s">
-        <v>165</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K2" s="21" t="s">
-        <v>166</v>
+        <v>7</v>
       </c>
       <c r="L2" s="21"/>
       <c r="M2" s="21"/>
@@ -5191,15 +5205,15 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
-        <v>177</v>
-      </c>
-      <c r="J15" s="22">
+        <v>18</v>
+      </c>
+      <c r="J15" s="20">
         <v>100000</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
-        <v>179</v>
+        <v>20</v>
       </c>
       <c r="J16">
         <v>70</v>
@@ -5207,7 +5221,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
-        <v>180</v>
+        <v>21</v>
       </c>
       <c r="J17">
         <v>90</v>
@@ -5215,18 +5229,18 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
-        <v>181</v>
+        <v>22</v>
       </c>
       <c r="J18" t="s">
-        <v>189</v>
+        <v>30</v>
       </c>
       <c r="K18" t="s">
-        <v>190</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
-        <v>185</v>
+        <v>26</v>
       </c>
       <c r="J22">
         <f>AVERAGE(E25,E53,E82,E111,E139)</f>
@@ -5235,13 +5249,13 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>162</v>
+        <v>3</v>
       </c>
       <c r="B23">
         <v>-1</v>
       </c>
       <c r="C23" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="D23">
         <v>1.08141</v>
@@ -5249,27 +5263,27 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="B24">
         <v>-1</v>
       </c>
       <c r="C24" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="D24">
         <v>1.0819000000000001</v>
       </c>
       <c r="E24" t="s">
-        <v>178</v>
+        <v>19</v>
       </c>
       <c r="I24" t="s">
-        <v>187</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>167</v>
+        <v>8</v>
       </c>
       <c r="B25">
         <f>+(B23)-(B24)</f>
@@ -5284,34 +5298,34 @@
         <v>49.000000000010147</v>
       </c>
       <c r="I25" t="s">
-        <v>188</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>168</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>169</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" s="20">
+        <v>11</v>
+      </c>
+      <c r="B29" s="19">
         <v>43847</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>162</v>
+        <v>3</v>
       </c>
       <c r="B51">
         <v>0.3</v>
       </c>
       <c r="C51" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="D51">
         <v>1.1134299999999999</v>
@@ -5319,24 +5333,24 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="B52">
         <v>0.3</v>
       </c>
       <c r="C52" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="D52">
         <v>1.11372</v>
       </c>
       <c r="E52" t="s">
-        <v>176</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>8</v>
       </c>
       <c r="B53">
         <f>+(B51)-(B52)</f>
@@ -5353,29 +5367,29 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>168</v>
+        <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>173</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>174</v>
-      </c>
-      <c r="B58" s="20">
+        <v>15</v>
+      </c>
+      <c r="B58" s="19">
         <v>43817</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>162</v>
+        <v>3</v>
       </c>
       <c r="B80">
         <v>-0.3</v>
       </c>
       <c r="C80" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="D80">
         <v>1.1112789999999999</v>
@@ -5383,24 +5397,24 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="B81">
         <v>-0.3</v>
       </c>
       <c r="C81" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="D81">
         <v>1.1136299999999999</v>
       </c>
       <c r="E81" t="s">
-        <v>176</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>167</v>
+        <v>8</v>
       </c>
       <c r="B82">
         <f>+(B80)-(B81)</f>
@@ -5417,29 +5431,29 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>168</v>
+        <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>175</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>182</v>
-      </c>
-      <c r="B87" s="20">
+        <v>23</v>
+      </c>
+      <c r="B87" s="19">
         <v>43784</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>162</v>
+        <v>3</v>
       </c>
       <c r="B109">
         <v>0.2</v>
       </c>
       <c r="C109" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="D109">
         <v>1.1016999999999999</v>
@@ -5447,24 +5461,24 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="B110">
         <v>0.1</v>
       </c>
       <c r="C110" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="D110">
         <v>1.1022799999999999</v>
       </c>
       <c r="E110" t="s">
-        <v>176</v>
+        <v>17</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>167</v>
+        <v>8</v>
       </c>
       <c r="B111">
         <f>+(B109)-(B110)</f>
@@ -5481,29 +5495,29 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>168</v>
+        <v>9</v>
       </c>
       <c r="B113" t="s">
-        <v>184</v>
+        <v>25</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>183</v>
-      </c>
-      <c r="B115" s="20">
+        <v>24</v>
+      </c>
+      <c r="B115" s="19">
         <v>43663</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>162</v>
+        <v>3</v>
       </c>
       <c r="B137">
         <v>0.1</v>
       </c>
       <c r="C137" t="s">
-        <v>171</v>
+        <v>12</v>
       </c>
       <c r="D137">
         <v>1.12107</v>
@@ -5511,24 +5525,24 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="B138">
         <v>0.2</v>
       </c>
       <c r="C138" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="D138">
         <v>1.12148</v>
       </c>
       <c r="E138" t="s">
-        <v>176</v>
+        <v>17</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>167</v>
+        <v>8</v>
       </c>
       <c r="B139">
         <f>+(B137)-(B138)</f>
@@ -5545,10 +5559,10 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>168</v>
+        <v>9</v>
       </c>
       <c r="B141" t="s">
-        <v>186</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>